<commit_message>
Archivos Análisis de la recolección de datos
</commit_message>
<xml_diff>
--- a/docs/trim1/levantamiento_informacion/1_recoleccion_informacion.xlsx
+++ b/docs/trim1/levantamiento_informacion/1_recoleccion_informacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="712" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="712" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja de Control" sheetId="5" r:id="rId1"/>
@@ -558,7 +558,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="34">
+  <fonts count="35">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -753,6 +753,14 @@
       <color rgb="FFFFFF00"/>
       <name val="Arial2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -798,7 +806,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="57">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -1572,13 +1580,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1814,6 +1836,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1854,34 +1907,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1903,6 +1928,36 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1912,15 +1967,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1930,26 +1976,26 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="4" borderId="53" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1957,18 +2003,6 @@
     <xf numFmtId="0" fontId="29" fillId="4" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="4" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1984,15 +2018,6 @@
     <xf numFmtId="0" fontId="30" fillId="6" borderId="52" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="4" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2038,12 +2063,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="57" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Excel_BuiltIn_Hyperlink" xfId="2"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -2100,7 +2129,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2200,8 +2228,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="327175448"/>
-        <c:axId val="327175832"/>
+        <c:axId val="324697584"/>
+        <c:axId val="324696800"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2282,11 +2310,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="327175448"/>
-        <c:axId val="327175832"/>
+        <c:axId val="324697584"/>
+        <c:axId val="324696800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="327175448"/>
+        <c:axId val="324697584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2329,7 +2357,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327175832"/>
+        <c:crossAx val="324696800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2337,7 +2365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="327175832"/>
+        <c:axId val="324696800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2388,7 +2416,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327175448"/>
+        <c:crossAx val="324697584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2523,7 +2551,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2707,12 +2734,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="327297464"/>
-        <c:axId val="327297848"/>
+        <c:axId val="324700328"/>
+        <c:axId val="324699544"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="327297464"/>
+        <c:axId val="324700328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2749,7 +2776,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327297848"/>
+        <c:crossAx val="324699544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2757,7 +2784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="327297848"/>
+        <c:axId val="324699544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2808,7 +2835,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327297464"/>
+        <c:crossAx val="324700328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2822,7 +2849,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2904,7 +2930,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3096,12 +3121,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="327382176"/>
-        <c:axId val="327384616"/>
+        <c:axId val="324698368"/>
+        <c:axId val="324698760"/>
         <c:axId val="0"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="327382176"/>
+        <c:axId val="324698368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3144,7 +3169,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327384616"/>
+        <c:crossAx val="324698760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3152,7 +3177,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="327384616"/>
+        <c:axId val="324698760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3203,7 +3228,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327382176"/>
+        <c:crossAx val="324698368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3217,7 +3242,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4950,7 +4974,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5004,7 +5028,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5058,7 +5082,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5112,7 +5136,7 @@
         <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5166,7 +5190,7 @@
         <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5220,7 +5244,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5364,7 +5388,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5718,55 +5742,55 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
     </row>
     <row r="7" spans="1:11" ht="30">
-      <c r="C7" s="120" t="s">
+      <c r="C7" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="121"/>
-      <c r="E7" s="122"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="103"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="C8" s="120" t="s">
+      <c r="C8" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="121"/>
-      <c r="E8" s="122"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="103"/>
     </row>
     <row r="10" spans="1:11" s="41" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="124"/>
-      <c r="B10" s="124"/>
-      <c r="C10" s="124"/>
-      <c r="D10" s="124"/>
-      <c r="E10" s="124"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="124"/>
-      <c r="H10" s="124"/>
-      <c r="I10" s="124"/>
-      <c r="J10" s="124"/>
-      <c r="K10" s="124"/>
+      <c r="A10" s="105"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickTop="1"/>
     <row r="13" spans="1:11" ht="30">
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
+      <c r="C13" s="104"/>
+      <c r="D13" s="104"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="104"/>
     </row>
     <row r="15" spans="1:11" ht="15" thickBot="1">
       <c r="B15" s="2"/>
@@ -5777,56 +5801,56 @@
       <c r="B16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="115" t="s">
+      <c r="C16" s="106" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="115"/>
-      <c r="E16" s="115"/>
-      <c r="F16" s="115"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="106"/>
+      <c r="F16" s="106"/>
     </row>
     <row r="17" spans="1:16" ht="18">
       <c r="B17" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="107" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="116"/>
-      <c r="E17" s="116"/>
-      <c r="F17" s="116"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="107"/>
     </row>
     <row r="18" spans="1:16" ht="18">
       <c r="B18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="117" t="s">
+      <c r="C18" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
+      <c r="D18" s="108"/>
+      <c r="E18" s="108"/>
+      <c r="F18" s="108"/>
     </row>
     <row r="19" spans="1:16" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A19" s="29"/>
       <c r="B19" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="116" t="s">
+      <c r="C19" s="107" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="116"/>
-      <c r="E19" s="116"/>
-      <c r="F19" s="116"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="107"/>
+      <c r="F19" s="107"/>
     </row>
     <row r="20" spans="1:16" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A20" s="29"/>
       <c r="B20" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="118" t="s">
+      <c r="C20" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="118"/>
+      <c r="D20" s="109"/>
       <c r="E20" s="7" t="s">
         <v>7</v>
       </c>
@@ -5836,13 +5860,13 @@
     </row>
     <row r="21" spans="1:16" ht="19.899999999999999" customHeight="1">
       <c r="A21" s="29"/>
-      <c r="B21" s="113" t="s">
+      <c r="B21" s="124" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="99" t="s">
+      <c r="C21" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="100"/>
+      <c r="D21" s="111"/>
       <c r="E21" s="9" t="s">
         <v>9</v>
       </c>
@@ -5852,9 +5876,9 @@
     </row>
     <row r="22" spans="1:16" ht="36.75" thickBot="1">
       <c r="A22" s="29"/>
-      <c r="B22" s="114"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="102"/>
+      <c r="B22" s="125"/>
+      <c r="C22" s="112"/>
+      <c r="D22" s="113"/>
       <c r="E22" s="10" t="s">
         <v>10</v>
       </c>
@@ -5884,10 +5908,10 @@
       <c r="C26" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="106" t="s">
+      <c r="D26" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="106"/>
+      <c r="E26" s="117"/>
       <c r="F26" s="16" t="s">
         <v>16</v>
       </c>
@@ -5899,10 +5923,10 @@
       <c r="C27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="107" t="s">
+      <c r="D27" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="107"/>
+      <c r="E27" s="118"/>
       <c r="F27" s="19" t="s">
         <v>42</v>
       </c>
@@ -5914,10 +5938,10 @@
       <c r="C28" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D28" s="107" t="s">
+      <c r="D28" s="118" t="s">
         <v>96</v>
       </c>
-      <c r="E28" s="107"/>
+      <c r="E28" s="118"/>
       <c r="F28" s="8" t="s">
         <v>109</v>
       </c>
@@ -5925,50 +5949,50 @@
     <row r="29" spans="1:16" ht="39.950000000000003" customHeight="1">
       <c r="B29" s="20"/>
       <c r="C29" s="21"/>
-      <c r="D29" s="108"/>
-      <c r="E29" s="109"/>
+      <c r="D29" s="119"/>
+      <c r="E29" s="120"/>
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="1:16" ht="39.950000000000003" customHeight="1">
       <c r="B30" s="20"/>
       <c r="C30" s="21"/>
-      <c r="D30" s="110"/>
-      <c r="E30" s="110"/>
+      <c r="D30" s="121"/>
+      <c r="E30" s="121"/>
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:16" ht="25.5" customHeight="1">
       <c r="B31" s="20"/>
       <c r="C31" s="21"/>
-      <c r="D31" s="110"/>
-      <c r="E31" s="110"/>
+      <c r="D31" s="121"/>
+      <c r="E31" s="121"/>
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:16" ht="24.95" customHeight="1">
       <c r="B32" s="20"/>
       <c r="C32" s="21"/>
-      <c r="D32" s="110"/>
-      <c r="E32" s="110"/>
+      <c r="D32" s="121"/>
+      <c r="E32" s="121"/>
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:13" ht="25.5" customHeight="1">
       <c r="B33" s="20"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="111"/>
-      <c r="E33" s="111"/>
+      <c r="D33" s="122"/>
+      <c r="E33" s="122"/>
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:13" ht="25.5" customHeight="1">
       <c r="B34" s="20"/>
       <c r="C34" s="21"/>
-      <c r="D34" s="111"/>
-      <c r="E34" s="111"/>
+      <c r="D34" s="122"/>
+      <c r="E34" s="122"/>
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:13" ht="25.5" customHeight="1" thickBot="1">
       <c r="B35" s="22"/>
       <c r="C35" s="23"/>
-      <c r="D35" s="112"/>
-      <c r="E35" s="112"/>
+      <c r="D35" s="123"/>
+      <c r="E35" s="123"/>
       <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1">
@@ -5982,34 +6006,34 @@
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="39" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B39" s="105" t="s">
+      <c r="B39" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="105"/>
-      <c r="D39" s="105"/>
-      <c r="E39" s="105"/>
-      <c r="F39" s="105"/>
+      <c r="C39" s="116"/>
+      <c r="D39" s="116"/>
+      <c r="E39" s="116"/>
+      <c r="F39" s="116"/>
     </row>
     <row r="40" spans="1:13" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B40" s="103" t="s">
+      <c r="B40" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="103"/>
-      <c r="D40" s="103"/>
-      <c r="E40" s="103"/>
-      <c r="F40" s="103"/>
+      <c r="C40" s="114"/>
+      <c r="D40" s="114"/>
+      <c r="E40" s="114"/>
+      <c r="F40" s="114"/>
       <c r="J40" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="25.5" customHeight="1">
-      <c r="B41" s="104" t="s">
+      <c r="B41" s="115" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="104"/>
-      <c r="D41" s="104"/>
-      <c r="E41" s="104"/>
-      <c r="F41" s="104"/>
+      <c r="C41" s="115"/>
+      <c r="D41" s="115"/>
+      <c r="E41" s="115"/>
+      <c r="F41" s="115"/>
     </row>
     <row r="42" spans="1:13" ht="25.5" customHeight="1">
       <c r="B42" s="25"/>
@@ -6326,18 +6350,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D22"/>
     <mergeCell ref="B40:F40"/>
     <mergeCell ref="B41:F41"/>
@@ -6353,6 +6365,18 @@
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A10:K10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="3.937007874015748E-2" bottom="3.937007874015748E-2" header="0" footer="0"/>
@@ -6387,56 +6411,56 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:10" s="41" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="A3" s="127"/>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127"/>
-      <c r="J3" s="127"/>
+      <c r="A3" s="128"/>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="128"/>
     </row>
     <row r="4" spans="1:10" s="42" customFormat="1" ht="20.25">
-      <c r="A4" s="128" t="s">
+      <c r="A4" s="129" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="128"/>
-      <c r="C4" s="128"/>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
-      <c r="H4" s="128"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="128"/>
+      <c r="B4" s="129"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
     </row>
     <row r="5" spans="1:10" s="42" customFormat="1" ht="20.25">
-      <c r="A5" s="128" t="s">
+      <c r="A5" s="129" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="128"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="128"/>
-      <c r="I5" s="128"/>
-      <c r="J5" s="128"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="129"/>
+      <c r="J5" s="129"/>
     </row>
     <row r="6" spans="1:10" s="41" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A6" s="124"/>
-      <c r="B6" s="124"/>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="124"/>
-      <c r="F6" s="124"/>
-      <c r="G6" s="124"/>
-      <c r="H6" s="124"/>
-      <c r="I6" s="124"/>
-      <c r="J6" s="124"/>
+      <c r="A6" s="105"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="105"/>
+      <c r="J6" s="105"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickTop="1"/>
     <row r="8" spans="1:10" ht="15" thickBot="1">
@@ -6476,7 +6500,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" s="36" customFormat="1" ht="60" customHeight="1">
-      <c r="B10" s="125" t="s">
+      <c r="B10" s="126" t="s">
         <v>47</v>
       </c>
       <c r="C10" s="67" t="s">
@@ -6502,7 +6526,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" s="36" customFormat="1" ht="42" customHeight="1">
-      <c r="B11" s="125"/>
+      <c r="B11" s="126"/>
       <c r="C11" s="67" t="s">
         <v>37</v>
       </c>
@@ -6526,7 +6550,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" customFormat="1" ht="69.95" customHeight="1">
-      <c r="B12" s="125" t="s">
+      <c r="B12" s="126" t="s">
         <v>83</v>
       </c>
       <c r="C12" s="67" t="s">
@@ -6552,7 +6576,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" customFormat="1" ht="45" customHeight="1" thickBot="1">
-      <c r="B13" s="126"/>
+      <c r="B13" s="127"/>
       <c r="C13" s="68" t="s">
         <v>37</v>
       </c>
@@ -6784,60 +6808,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
     </row>
     <row r="7" spans="1:11" ht="30">
-      <c r="A7" s="120" t="s">
+      <c r="A7" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="121"/>
-      <c r="C7" s="121"/>
-      <c r="D7" s="121"/>
-      <c r="E7" s="121"/>
-      <c r="F7" s="121"/>
-      <c r="G7" s="121"/>
-      <c r="H7" s="121"/>
-      <c r="I7" s="121"/>
-      <c r="J7" s="121"/>
-      <c r="K7" s="122"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="102"/>
+      <c r="I7" s="102"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="103"/>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="120" t="s">
+      <c r="A8" s="101" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="121"/>
-      <c r="C8" s="121"/>
-      <c r="D8" s="121"/>
-      <c r="E8" s="121"/>
-      <c r="F8" s="121"/>
-      <c r="G8" s="121"/>
-      <c r="H8" s="121"/>
-      <c r="I8" s="121"/>
-      <c r="J8" s="121"/>
-      <c r="K8" s="122"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="103"/>
     </row>
     <row r="10" spans="1:11" s="41" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="124"/>
-      <c r="B10" s="124"/>
-      <c r="C10" s="124"/>
-      <c r="D10" s="124"/>
-      <c r="E10" s="124"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="124"/>
-      <c r="H10" s="124"/>
-      <c r="I10" s="124"/>
-      <c r="J10" s="124"/>
-      <c r="K10" s="124"/>
+      <c r="A10" s="105"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickTop="1"/>
     <row r="12" spans="1:11">
@@ -7048,8 +7072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IW41"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -7072,60 +7096,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="A7" s="120" t="s">
+      <c r="A7" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="121"/>
-      <c r="C7" s="121"/>
-      <c r="D7" s="121"/>
-      <c r="E7" s="121"/>
-      <c r="F7" s="121"/>
-      <c r="G7" s="121"/>
-      <c r="H7" s="121"/>
-      <c r="I7" s="121"/>
-      <c r="J7" s="121"/>
-      <c r="K7" s="122"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="102"/>
+      <c r="I7" s="102"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="103"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="A8" s="120" t="s">
+      <c r="A8" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="121"/>
-      <c r="C8" s="121"/>
-      <c r="D8" s="121"/>
-      <c r="E8" s="121"/>
-      <c r="F8" s="121"/>
-      <c r="G8" s="121"/>
-      <c r="H8" s="121"/>
-      <c r="I8" s="121"/>
-      <c r="J8" s="121"/>
-      <c r="K8" s="122"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="103"/>
     </row>
     <row r="10" spans="1:257" s="41" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="124"/>
-      <c r="B10" s="124"/>
-      <c r="C10" s="124"/>
-      <c r="D10" s="124"/>
-      <c r="E10" s="124"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="124"/>
-      <c r="H10" s="124"/>
-      <c r="I10" s="124"/>
-      <c r="J10" s="124"/>
-      <c r="K10" s="124"/>
+      <c r="A10" s="105"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="105"/>
     </row>
     <row r="11" spans="1:257" ht="15" thickTop="1"/>
     <row r="12" spans="1:257">
@@ -7139,7 +7163,7 @@
     <row r="15" spans="1:257" s="1" customFormat="1" ht="50.1" customHeight="1" thickBot="1">
       <c r="A15" s="29"/>
       <c r="B15" s="45"/>
-      <c r="C15" s="50" t="s">
+      <c r="C15" s="178" t="s">
         <v>50</v>
       </c>
       <c r="D15" s="51" t="s">
@@ -7157,7 +7181,7 @@
     <row r="16" spans="1:257" s="1" customFormat="1" ht="120" customHeight="1">
       <c r="A16" s="29"/>
       <c r="B16" s="46"/>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="179" t="s">
         <v>64</v>
       </c>
       <c r="D16" s="49">
@@ -7216,7 +7240,7 @@
       <c r="D19" s="84">
         <v>44999</v>
       </c>
-      <c r="E19" s="177" t="s">
+      <c r="E19" s="99" t="s">
         <v>56</v>
       </c>
       <c r="F19" s="34"/>
@@ -7373,10 +7397,13 @@
     <mergeCell ref="A7:K7"/>
     <mergeCell ref="A8:K8"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C16" r:id="rId1"/>
+  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="3.937007874015748E-2" bottom="3.937007874015748E-2" header="0" footer="0"/>
-  <pageSetup scale="45" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup scale="45" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -7385,7 +7412,7 @@
   <dimension ref="A2:IW41"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -7410,60 +7437,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:253">
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
     </row>
     <row r="6" spans="1:253">
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
     </row>
     <row r="7" spans="1:253" ht="30">
-      <c r="A7" s="120" t="s">
+      <c r="A7" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="121"/>
-      <c r="C7" s="121"/>
-      <c r="D7" s="121"/>
-      <c r="E7" s="121"/>
-      <c r="F7" s="121"/>
-      <c r="G7" s="121"/>
-      <c r="H7" s="121"/>
-      <c r="I7" s="121"/>
-      <c r="J7" s="121"/>
-      <c r="K7" s="122"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="102"/>
+      <c r="I7" s="102"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="103"/>
     </row>
     <row r="8" spans="1:253" ht="30">
-      <c r="A8" s="120" t="s">
+      <c r="A8" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="121"/>
-      <c r="C8" s="121"/>
-      <c r="D8" s="121"/>
-      <c r="E8" s="121"/>
-      <c r="F8" s="121"/>
-      <c r="G8" s="121"/>
-      <c r="H8" s="121"/>
-      <c r="I8" s="121"/>
-      <c r="J8" s="121"/>
-      <c r="K8" s="122"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="103"/>
     </row>
     <row r="10" spans="1:253" s="41" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="141"/>
-      <c r="B10" s="141"/>
-      <c r="C10" s="141"/>
-      <c r="D10" s="141"/>
-      <c r="E10" s="141"/>
-      <c r="F10" s="141"/>
-      <c r="G10" s="141"/>
-      <c r="H10" s="141"/>
-      <c r="I10" s="141"/>
-      <c r="J10" s="141"/>
-      <c r="K10" s="141"/>
+      <c r="A10" s="136"/>
+      <c r="B10" s="136"/>
+      <c r="C10" s="136"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="136"/>
+      <c r="F10" s="136"/>
+      <c r="G10" s="136"/>
+      <c r="H10" s="136"/>
+      <c r="I10" s="136"/>
+      <c r="J10" s="136"/>
+      <c r="K10" s="136"/>
     </row>
     <row r="11" spans="1:253" ht="15" thickTop="1"/>
     <row r="12" spans="1:253">
@@ -7475,24 +7502,24 @@
     </row>
     <row r="14" spans="1:253" s="58" customFormat="1" ht="30" customHeight="1">
       <c r="A14" s="57"/>
-      <c r="B14" s="132" t="s">
+      <c r="B14" s="143" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="133"/>
-      <c r="D14" s="133"/>
-      <c r="E14" s="133"/>
-      <c r="F14" s="134"/>
+      <c r="C14" s="144"/>
+      <c r="D14" s="144"/>
+      <c r="E14" s="144"/>
+      <c r="F14" s="145"/>
       <c r="G14" s="57"/>
-      <c r="H14" s="142"/>
-      <c r="I14" s="143"/>
-      <c r="J14" s="143"/>
-      <c r="K14" s="143"/>
-      <c r="L14" s="143"/>
-      <c r="M14" s="143"/>
-      <c r="N14" s="143"/>
-      <c r="O14" s="143"/>
-      <c r="P14" s="143"/>
-      <c r="Q14" s="144"/>
+      <c r="H14" s="137"/>
+      <c r="I14" s="138"/>
+      <c r="J14" s="138"/>
+      <c r="K14" s="138"/>
+      <c r="L14" s="138"/>
+      <c r="M14" s="138"/>
+      <c r="N14" s="138"/>
+      <c r="O14" s="138"/>
+      <c r="P14" s="138"/>
+      <c r="Q14" s="139"/>
       <c r="R14" s="57"/>
       <c r="S14" s="57"/>
       <c r="T14" s="57"/>
@@ -7731,13 +7758,13 @@
     </row>
     <row r="15" spans="1:253" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A15" s="29"/>
-      <c r="B15" s="145" t="s">
+      <c r="B15" s="140" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="146"/>
-      <c r="D15" s="146"/>
-      <c r="E15" s="146"/>
-      <c r="F15" s="147"/>
+      <c r="C15" s="141"/>
+      <c r="D15" s="141"/>
+      <c r="E15" s="141"/>
+      <c r="F15" s="142"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="IS15" s="2"/>
@@ -7745,9 +7772,9 @@
     <row r="16" spans="1:253" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A16" s="29"/>
       <c r="B16" s="59"/>
-      <c r="C16" s="135"/>
-      <c r="D16" s="136"/>
-      <c r="E16" s="137"/>
+      <c r="C16" s="133"/>
+      <c r="D16" s="134"/>
+      <c r="E16" s="135"/>
       <c r="F16" s="93"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
@@ -7756,12 +7783,12 @@
     <row r="17" spans="1:257" s="1" customFormat="1" ht="24.95" customHeight="1">
       <c r="A17" s="29"/>
       <c r="B17" s="61"/>
-      <c r="C17" s="135" t="s">
+      <c r="C17" s="133" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="136"/>
-      <c r="E17" s="136"/>
-      <c r="F17" s="137"/>
+      <c r="D17" s="134"/>
+      <c r="E17" s="134"/>
+      <c r="F17" s="135"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="IS17" s="2"/>
@@ -7769,9 +7796,9 @@
     <row r="18" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A18" s="29"/>
       <c r="B18" s="61"/>
-      <c r="C18" s="138"/>
-      <c r="D18" s="139"/>
-      <c r="E18" s="140"/>
+      <c r="C18" s="146"/>
+      <c r="D18" s="147"/>
+      <c r="E18" s="148"/>
       <c r="F18" s="60"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
@@ -7780,118 +7807,118 @@
     <row r="19" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A19" s="29"/>
       <c r="B19" s="61"/>
-      <c r="C19" s="129" t="s">
+      <c r="C19" s="130" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="130"/>
-      <c r="E19" s="130"/>
-      <c r="F19" s="131"/>
+      <c r="D19" s="131"/>
+      <c r="E19" s="131"/>
+      <c r="F19" s="132"/>
       <c r="IS19" s="2"/>
     </row>
     <row r="20" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A20" s="29"/>
       <c r="B20" s="61"/>
-      <c r="C20" s="129" t="s">
+      <c r="C20" s="130" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="130"/>
-      <c r="E20" s="130"/>
-      <c r="F20" s="131"/>
+      <c r="D20" s="131"/>
+      <c r="E20" s="131"/>
+      <c r="F20" s="132"/>
       <c r="IS20" s="2"/>
     </row>
     <row r="21" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A21" s="29"/>
       <c r="B21" s="61"/>
-      <c r="C21" s="129" t="s">
+      <c r="C21" s="130" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="130"/>
-      <c r="E21" s="130"/>
-      <c r="F21" s="131"/>
+      <c r="D21" s="131"/>
+      <c r="E21" s="131"/>
+      <c r="F21" s="132"/>
       <c r="IS21" s="2"/>
     </row>
     <row r="22" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A22" s="29"/>
       <c r="B22" s="61"/>
-      <c r="C22" s="129" t="s">
+      <c r="C22" s="130" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="130"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="131"/>
+      <c r="D22" s="131"/>
+      <c r="E22" s="131"/>
+      <c r="F22" s="132"/>
       <c r="IS22" s="2"/>
     </row>
     <row r="23" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A23" s="29"/>
       <c r="B23" s="61"/>
-      <c r="C23" s="129" t="s">
+      <c r="C23" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="130"/>
-      <c r="E23" s="130"/>
-      <c r="F23" s="131"/>
+      <c r="D23" s="131"/>
+      <c r="E23" s="131"/>
+      <c r="F23" s="132"/>
       <c r="IS23" s="2"/>
     </row>
     <row r="24" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A24" s="29"/>
       <c r="B24" s="61"/>
-      <c r="C24" s="129" t="s">
+      <c r="C24" s="130" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="130"/>
-      <c r="E24" s="130"/>
-      <c r="F24" s="131"/>
+      <c r="D24" s="131"/>
+      <c r="E24" s="131"/>
+      <c r="F24" s="132"/>
       <c r="IS24" s="2"/>
     </row>
     <row r="25" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A25" s="29"/>
       <c r="B25" s="61"/>
-      <c r="C25" s="129" t="s">
+      <c r="C25" s="130" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="130"/>
-      <c r="E25" s="130"/>
-      <c r="F25" s="131"/>
+      <c r="D25" s="131"/>
+      <c r="E25" s="131"/>
+      <c r="F25" s="132"/>
       <c r="IS25" s="2"/>
     </row>
     <row r="26" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A26" s="29"/>
       <c r="B26" s="61"/>
-      <c r="C26" s="129" t="s">
+      <c r="C26" s="130" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="130"/>
-      <c r="E26" s="130"/>
-      <c r="F26" s="131"/>
+      <c r="D26" s="131"/>
+      <c r="E26" s="131"/>
+      <c r="F26" s="132"/>
       <c r="IS26" s="2"/>
     </row>
     <row r="27" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A27" s="29"/>
       <c r="B27" s="61"/>
-      <c r="C27" s="129" t="s">
+      <c r="C27" s="130" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="130"/>
-      <c r="E27" s="130"/>
-      <c r="F27" s="131"/>
+      <c r="D27" s="131"/>
+      <c r="E27" s="131"/>
+      <c r="F27" s="132"/>
       <c r="IS27" s="2"/>
     </row>
     <row r="28" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="B28" s="61"/>
-      <c r="C28" s="138"/>
-      <c r="D28" s="139"/>
-      <c r="E28" s="139"/>
-      <c r="F28" s="140"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="147"/>
+      <c r="E28" s="147"/>
+      <c r="F28" s="148"/>
       <c r="IS28" s="2"/>
     </row>
     <row r="29" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="B29" s="61"/>
-      <c r="C29" s="135" t="s">
+      <c r="C29" s="133" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="136"/>
-      <c r="E29" s="136"/>
-      <c r="F29" s="137"/>
+      <c r="D29" s="134"/>
+      <c r="E29" s="134"/>
+      <c r="F29" s="135"/>
       <c r="IS29" s="2"/>
     </row>
     <row r="30" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
@@ -7904,44 +7931,44 @@
     </row>
     <row r="31" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="B31" s="66"/>
-      <c r="C31" s="129" t="s">
+      <c r="C31" s="130" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="130"/>
-      <c r="E31" s="130"/>
-      <c r="F31" s="131"/>
+      <c r="D31" s="131"/>
+      <c r="E31" s="131"/>
+      <c r="F31" s="132"/>
       <c r="IW31" s="2"/>
     </row>
     <row r="32" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="B32" s="62"/>
-      <c r="C32" s="129" t="s">
+      <c r="C32" s="130" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="130"/>
-      <c r="E32" s="130"/>
-      <c r="F32" s="131"/>
+      <c r="D32" s="131"/>
+      <c r="E32" s="131"/>
+      <c r="F32" s="132"/>
       <c r="J32" s="34"/>
       <c r="IW32" s="2"/>
     </row>
     <row r="33" spans="2:257" s="1" customFormat="1" ht="15.75">
       <c r="B33" s="66"/>
-      <c r="C33" s="129" t="s">
+      <c r="C33" s="130" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="130"/>
-      <c r="E33" s="130"/>
-      <c r="F33" s="131"/>
+      <c r="D33" s="131"/>
+      <c r="E33" s="131"/>
+      <c r="F33" s="132"/>
       <c r="J33" s="34"/>
       <c r="IW33" s="2"/>
     </row>
     <row r="34" spans="2:257" s="1" customFormat="1" ht="15.75">
       <c r="B34" s="62"/>
-      <c r="C34" s="129" t="s">
+      <c r="C34" s="130" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="130"/>
-      <c r="E34" s="130"/>
-      <c r="F34" s="131"/>
+      <c r="D34" s="131"/>
+      <c r="E34" s="131"/>
+      <c r="F34" s="132"/>
       <c r="IW34" s="2"/>
     </row>
     <row r="35" spans="2:257" s="1" customFormat="1">
@@ -7993,17 +8020,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="A7:K7"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="H14:Q14"/>
-    <mergeCell ref="B15:F15"/>
     <mergeCell ref="C34:F34"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="C17:F17"/>
@@ -8020,6 +8036,17 @@
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="C31:F31"/>
     <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="H14:Q14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="A7:K7"/>
+    <mergeCell ref="A8:K8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="3.937007874015748E-2" bottom="3.937007874015748E-2" header="0" footer="0"/>
@@ -8055,60 +8082,60 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="A7" s="120" t="s">
+      <c r="A7" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="121"/>
-      <c r="C7" s="121"/>
-      <c r="D7" s="121"/>
-      <c r="E7" s="121"/>
-      <c r="F7" s="121"/>
-      <c r="G7" s="121"/>
-      <c r="H7" s="121"/>
-      <c r="I7" s="121"/>
-      <c r="J7" s="121"/>
-      <c r="K7" s="122"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="102"/>
+      <c r="I7" s="102"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="103"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="A8" s="120" t="s">
+      <c r="A8" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="121"/>
-      <c r="C8" s="121"/>
-      <c r="D8" s="121"/>
-      <c r="E8" s="121"/>
-      <c r="F8" s="121"/>
-      <c r="G8" s="121"/>
-      <c r="H8" s="121"/>
-      <c r="I8" s="121"/>
-      <c r="J8" s="121"/>
-      <c r="K8" s="122"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="103"/>
     </row>
     <row r="10" spans="1:257" s="41" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="124"/>
-      <c r="B10" s="124"/>
-      <c r="C10" s="124"/>
-      <c r="D10" s="124"/>
-      <c r="E10" s="124"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="124"/>
-      <c r="H10" s="124"/>
-      <c r="I10" s="124"/>
-      <c r="J10" s="124"/>
-      <c r="K10" s="124"/>
+      <c r="A10" s="105"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="105"/>
     </row>
     <row r="11" spans="1:257" ht="15" thickTop="1"/>
     <row r="12" spans="1:257">
@@ -8129,47 +8156,47 @@
     </row>
     <row r="16" spans="1:257" s="1" customFormat="1" ht="50.1" customHeight="1">
       <c r="A16" s="29"/>
-      <c r="B16" s="156" t="s">
+      <c r="B16" s="160" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="157"/>
-      <c r="D16" s="158"/>
+      <c r="C16" s="161"/>
+      <c r="D16" s="162"/>
       <c r="E16" s="87"/>
-      <c r="F16" s="159" t="s">
+      <c r="F16" s="149" t="s">
         <v>97</v>
       </c>
-      <c r="G16" s="160"/>
-      <c r="H16" s="161"/>
+      <c r="G16" s="150"/>
+      <c r="H16" s="151"/>
       <c r="I16" s="34"/>
-      <c r="K16" s="159" t="s">
+      <c r="K16" s="149" t="s">
         <v>103</v>
       </c>
-      <c r="L16" s="160"/>
-      <c r="M16" s="161"/>
+      <c r="L16" s="150"/>
+      <c r="M16" s="151"/>
       <c r="IW16" s="2"/>
     </row>
     <row r="17" spans="1:257" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A17" s="29"/>
-      <c r="B17" s="150" t="s">
+      <c r="B17" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="151"/>
+      <c r="C17" s="153"/>
       <c r="D17" s="88" t="s">
         <v>87</v>
       </c>
       <c r="E17" s="87"/>
-      <c r="F17" s="150" t="s">
+      <c r="F17" s="152" t="s">
         <v>90</v>
       </c>
-      <c r="G17" s="151"/>
+      <c r="G17" s="153"/>
       <c r="H17" s="88" t="s">
         <v>89</v>
       </c>
       <c r="I17" s="34"/>
-      <c r="K17" s="150" t="s">
+      <c r="K17" s="152" t="s">
         <v>90</v>
       </c>
-      <c r="L17" s="151"/>
+      <c r="L17" s="153"/>
       <c r="M17" s="96" t="s">
         <v>106</v>
       </c>
@@ -8177,26 +8204,26 @@
     </row>
     <row r="18" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A18" s="29"/>
-      <c r="B18" s="152" t="s">
+      <c r="B18" s="154" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="153"/>
+      <c r="C18" s="155"/>
       <c r="D18" s="89">
         <v>0.75</v>
       </c>
       <c r="E18" s="87"/>
-      <c r="F18" s="152" t="s">
+      <c r="F18" s="154" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="153"/>
+      <c r="G18" s="155"/>
       <c r="H18" s="89">
         <v>0.65</v>
       </c>
       <c r="I18" s="34"/>
-      <c r="K18" s="152" t="s">
+      <c r="K18" s="154" t="s">
         <v>104</v>
       </c>
-      <c r="L18" s="153"/>
+      <c r="L18" s="155"/>
       <c r="M18" s="89">
         <v>0.85</v>
       </c>
@@ -8204,26 +8231,26 @@
     </row>
     <row r="19" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A19" s="29"/>
-      <c r="B19" s="154" t="s">
+      <c r="B19" s="158" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="155"/>
+      <c r="C19" s="159"/>
       <c r="D19" s="90">
         <v>0.25</v>
       </c>
       <c r="E19" s="87"/>
-      <c r="F19" s="152" t="s">
+      <c r="F19" s="154" t="s">
         <v>93</v>
       </c>
-      <c r="G19" s="153"/>
+      <c r="G19" s="155"/>
       <c r="H19" s="89">
         <v>0.1</v>
       </c>
       <c r="I19" s="34"/>
-      <c r="K19" s="152" t="s">
+      <c r="K19" s="154" t="s">
         <v>105</v>
       </c>
-      <c r="L19" s="153"/>
+      <c r="L19" s="155"/>
       <c r="M19" s="89">
         <v>0.15</v>
       </c>
@@ -8235,10 +8262,10 @@
       <c r="C20" s="39"/>
       <c r="D20" s="39"/>
       <c r="E20" s="29"/>
-      <c r="F20" s="148" t="s">
+      <c r="F20" s="156" t="s">
         <v>92</v>
       </c>
-      <c r="G20" s="149"/>
+      <c r="G20" s="157"/>
       <c r="H20" s="92">
         <v>0.25</v>
       </c>
@@ -8356,6 +8383,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="A7:K7"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B16:D16"/>
     <mergeCell ref="K16:M16"/>
     <mergeCell ref="K17:L17"/>
     <mergeCell ref="K18:L18"/>
@@ -8364,17 +8402,6 @@
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="A7:K7"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="3.937007874015748E-2" bottom="3.937007874015748E-2" header="0" footer="0"/>
@@ -8387,7 +8414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B14" sqref="B14:I15"/>
     </sheetView>
   </sheetViews>
@@ -8430,56 +8457,56 @@
       <c r="IV4" s="1"/>
     </row>
     <row r="5" spans="1:256">
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
       <c r="IT5" s="1"/>
       <c r="IU5" s="1"/>
       <c r="IV5" s="1"/>
     </row>
     <row r="6" spans="1:256">
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
       <c r="IT6" s="1"/>
       <c r="IU6" s="1"/>
       <c r="IV6" s="1"/>
     </row>
     <row r="7" spans="1:256" ht="30">
-      <c r="A7" s="120" t="s">
+      <c r="A7" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="121"/>
-      <c r="C7" s="121"/>
-      <c r="D7" s="121"/>
-      <c r="E7" s="121"/>
-      <c r="F7" s="121"/>
-      <c r="G7" s="121"/>
-      <c r="H7" s="121"/>
-      <c r="I7" s="121"/>
-      <c r="J7" s="121"/>
-      <c r="K7" s="122"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="102"/>
+      <c r="I7" s="102"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="103"/>
       <c r="IT7" s="1"/>
       <c r="IU7" s="1"/>
       <c r="IV7" s="1"/>
     </row>
     <row r="8" spans="1:256" ht="30">
-      <c r="A8" s="120" t="s">
+      <c r="A8" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="121"/>
-      <c r="C8" s="121"/>
-      <c r="D8" s="121"/>
-      <c r="E8" s="121"/>
-      <c r="F8" s="121"/>
-      <c r="G8" s="121"/>
-      <c r="H8" s="121"/>
-      <c r="I8" s="121"/>
-      <c r="J8" s="121"/>
-      <c r="K8" s="122"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="103"/>
       <c r="IT8" s="1"/>
       <c r="IU8" s="1"/>
       <c r="IV8" s="1"/>
@@ -8490,17 +8517,17 @@
       <c r="IV9" s="1"/>
     </row>
     <row r="10" spans="1:256" s="41" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="124"/>
-      <c r="B10" s="124"/>
-      <c r="C10" s="124"/>
-      <c r="D10" s="124"/>
-      <c r="E10" s="124"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="124"/>
-      <c r="H10" s="124"/>
-      <c r="I10" s="124"/>
-      <c r="J10" s="124"/>
-      <c r="K10" s="124"/>
+      <c r="A10" s="105"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="105"/>
     </row>
     <row r="11" spans="1:256" ht="15" thickTop="1">
       <c r="IT11" s="1"/>
@@ -8522,44 +8549,44 @@
     </row>
     <row r="14" spans="1:256" ht="30" customHeight="1">
       <c r="A14" s="29"/>
-      <c r="B14" s="168" t="s">
+      <c r="B14" s="169" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="169"/>
-      <c r="D14" s="169"/>
-      <c r="E14" s="169"/>
-      <c r="F14" s="169"/>
-      <c r="G14" s="169"/>
-      <c r="H14" s="169"/>
-      <c r="I14" s="170"/>
+      <c r="C14" s="170"/>
+      <c r="D14" s="170"/>
+      <c r="E14" s="170"/>
+      <c r="F14" s="170"/>
+      <c r="G14" s="170"/>
+      <c r="H14" s="170"/>
+      <c r="I14" s="171"/>
       <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:256" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A15" s="29"/>
-      <c r="B15" s="171"/>
-      <c r="C15" s="172"/>
-      <c r="D15" s="172"/>
-      <c r="E15" s="172"/>
-      <c r="F15" s="172"/>
-      <c r="G15" s="172"/>
-      <c r="H15" s="172"/>
-      <c r="I15" s="173"/>
+      <c r="B15" s="172"/>
+      <c r="C15" s="173"/>
+      <c r="D15" s="173"/>
+      <c r="E15" s="173"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="174"/>
       <c r="J15" s="34"/>
       <c r="K15" s="13"/>
       <c r="IT15" s="2"/>
     </row>
     <row r="16" spans="1:256" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A16" s="29"/>
-      <c r="B16" s="174" t="s">
+      <c r="B16" s="175" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="175"/>
-      <c r="D16" s="175"/>
-      <c r="E16" s="175"/>
-      <c r="F16" s="175"/>
-      <c r="G16" s="175"/>
-      <c r="H16" s="175"/>
-      <c r="I16" s="176"/>
+      <c r="C16" s="176"/>
+      <c r="D16" s="176"/>
+      <c r="E16" s="176"/>
+      <c r="F16" s="176"/>
+      <c r="G16" s="176"/>
+      <c r="H16" s="176"/>
+      <c r="I16" s="177"/>
       <c r="J16" s="94"/>
       <c r="K16" s="94"/>
       <c r="L16" s="94"/>
@@ -8568,194 +8595,194 @@
     </row>
     <row r="17" spans="1:254" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A17" s="29"/>
-      <c r="B17" s="174"/>
-      <c r="C17" s="175"/>
-      <c r="D17" s="175"/>
-      <c r="E17" s="175"/>
-      <c r="F17" s="175"/>
-      <c r="G17" s="175"/>
-      <c r="H17" s="175"/>
-      <c r="I17" s="176"/>
+      <c r="B17" s="175"/>
+      <c r="C17" s="176"/>
+      <c r="D17" s="176"/>
+      <c r="E17" s="176"/>
+      <c r="F17" s="176"/>
+      <c r="G17" s="176"/>
+      <c r="H17" s="176"/>
+      <c r="I17" s="177"/>
       <c r="J17" s="34"/>
       <c r="K17" s="13"/>
       <c r="IT17" s="2"/>
     </row>
     <row r="18" spans="1:254" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A18" s="29"/>
-      <c r="B18" s="174"/>
-      <c r="C18" s="175"/>
-      <c r="D18" s="175"/>
-      <c r="E18" s="175"/>
-      <c r="F18" s="175"/>
-      <c r="G18" s="175"/>
-      <c r="H18" s="175"/>
-      <c r="I18" s="176"/>
+      <c r="B18" s="175"/>
+      <c r="C18" s="176"/>
+      <c r="D18" s="176"/>
+      <c r="E18" s="176"/>
+      <c r="F18" s="176"/>
+      <c r="G18" s="176"/>
+      <c r="H18" s="176"/>
+      <c r="I18" s="177"/>
       <c r="J18" s="34"/>
       <c r="K18" s="13"/>
       <c r="IT18" s="2"/>
     </row>
     <row r="19" spans="1:254" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A19" s="29"/>
-      <c r="B19" s="174"/>
-      <c r="C19" s="175"/>
-      <c r="D19" s="175"/>
-      <c r="E19" s="175"/>
-      <c r="F19" s="175"/>
-      <c r="G19" s="175"/>
-      <c r="H19" s="175"/>
-      <c r="I19" s="176"/>
+      <c r="B19" s="175"/>
+      <c r="C19" s="176"/>
+      <c r="D19" s="176"/>
+      <c r="E19" s="176"/>
+      <c r="F19" s="176"/>
+      <c r="G19" s="176"/>
+      <c r="H19" s="176"/>
+      <c r="I19" s="177"/>
       <c r="J19" s="34"/>
       <c r="IT19" s="2"/>
     </row>
     <row r="20" spans="1:254" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A20" s="29"/>
-      <c r="B20" s="171" t="s">
+      <c r="B20" s="172" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="172"/>
-      <c r="D20" s="172"/>
-      <c r="E20" s="172"/>
-      <c r="F20" s="172"/>
-      <c r="G20" s="172"/>
-      <c r="H20" s="172"/>
-      <c r="I20" s="173"/>
+      <c r="C20" s="173"/>
+      <c r="D20" s="173"/>
+      <c r="E20" s="173"/>
+      <c r="F20" s="173"/>
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="174"/>
       <c r="J20" s="34"/>
       <c r="IT20" s="2"/>
     </row>
     <row r="21" spans="1:254" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A21" s="29"/>
-      <c r="B21" s="171"/>
-      <c r="C21" s="172"/>
-      <c r="D21" s="172"/>
-      <c r="E21" s="172"/>
-      <c r="F21" s="172"/>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="173"/>
+      <c r="B21" s="172"/>
+      <c r="C21" s="173"/>
+      <c r="D21" s="173"/>
+      <c r="E21" s="173"/>
+      <c r="F21" s="173"/>
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="174"/>
       <c r="J21" s="34"/>
       <c r="IT21" s="2"/>
     </row>
     <row r="22" spans="1:254" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A22" s="29"/>
-      <c r="B22" s="162" t="s">
+      <c r="B22" s="163" t="s">
         <v>108</v>
       </c>
-      <c r="C22" s="163"/>
-      <c r="D22" s="163"/>
-      <c r="E22" s="163"/>
-      <c r="F22" s="163"/>
-      <c r="G22" s="163"/>
-      <c r="H22" s="163"/>
-      <c r="I22" s="164"/>
+      <c r="C22" s="164"/>
+      <c r="D22" s="164"/>
+      <c r="E22" s="164"/>
+      <c r="F22" s="164"/>
+      <c r="G22" s="164"/>
+      <c r="H22" s="164"/>
+      <c r="I22" s="165"/>
       <c r="J22" s="34"/>
       <c r="IT22" s="2"/>
     </row>
     <row r="23" spans="1:254" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A23" s="29"/>
-      <c r="B23" s="162"/>
-      <c r="C23" s="163"/>
-      <c r="D23" s="163"/>
-      <c r="E23" s="163"/>
-      <c r="F23" s="163"/>
-      <c r="G23" s="163"/>
-      <c r="H23" s="163"/>
-      <c r="I23" s="164"/>
+      <c r="B23" s="163"/>
+      <c r="C23" s="164"/>
+      <c r="D23" s="164"/>
+      <c r="E23" s="164"/>
+      <c r="F23" s="164"/>
+      <c r="G23" s="164"/>
+      <c r="H23" s="164"/>
+      <c r="I23" s="165"/>
       <c r="J23" s="34"/>
       <c r="IT23" s="2"/>
     </row>
     <row r="24" spans="1:254" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A24" s="29"/>
-      <c r="B24" s="162"/>
-      <c r="C24" s="163"/>
-      <c r="D24" s="163"/>
-      <c r="E24" s="163"/>
-      <c r="F24" s="163"/>
-      <c r="G24" s="163"/>
-      <c r="H24" s="163"/>
-      <c r="I24" s="164"/>
+      <c r="B24" s="163"/>
+      <c r="C24" s="164"/>
+      <c r="D24" s="164"/>
+      <c r="E24" s="164"/>
+      <c r="F24" s="164"/>
+      <c r="G24" s="164"/>
+      <c r="H24" s="164"/>
+      <c r="I24" s="165"/>
       <c r="J24" s="34"/>
       <c r="IT24" s="2"/>
     </row>
     <row r="25" spans="1:254" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A25" s="29"/>
-      <c r="B25" s="171" t="s">
+      <c r="B25" s="172" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="172"/>
-      <c r="D25" s="172"/>
-      <c r="E25" s="172"/>
-      <c r="F25" s="172"/>
-      <c r="G25" s="172"/>
-      <c r="H25" s="172"/>
-      <c r="I25" s="173"/>
+      <c r="C25" s="173"/>
+      <c r="D25" s="173"/>
+      <c r="E25" s="173"/>
+      <c r="F25" s="173"/>
+      <c r="G25" s="173"/>
+      <c r="H25" s="173"/>
+      <c r="I25" s="174"/>
       <c r="J25" s="34"/>
       <c r="IT25" s="2"/>
     </row>
     <row r="26" spans="1:254" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A26" s="29"/>
-      <c r="B26" s="171"/>
-      <c r="C26" s="172"/>
-      <c r="D26" s="172"/>
-      <c r="E26" s="172"/>
-      <c r="F26" s="172"/>
-      <c r="G26" s="172"/>
-      <c r="H26" s="172"/>
-      <c r="I26" s="173"/>
+      <c r="B26" s="172"/>
+      <c r="C26" s="173"/>
+      <c r="D26" s="173"/>
+      <c r="E26" s="173"/>
+      <c r="F26" s="173"/>
+      <c r="G26" s="173"/>
+      <c r="H26" s="173"/>
+      <c r="I26" s="174"/>
       <c r="J26" s="34"/>
       <c r="IT26" s="2"/>
     </row>
     <row r="27" spans="1:254" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A27" s="29"/>
-      <c r="B27" s="162" t="s">
+      <c r="B27" s="163" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="163"/>
-      <c r="D27" s="163"/>
-      <c r="E27" s="163"/>
-      <c r="F27" s="163"/>
-      <c r="G27" s="163"/>
-      <c r="H27" s="163"/>
-      <c r="I27" s="164"/>
+      <c r="C27" s="164"/>
+      <c r="D27" s="164"/>
+      <c r="E27" s="164"/>
+      <c r="F27" s="164"/>
+      <c r="G27" s="164"/>
+      <c r="H27" s="164"/>
+      <c r="I27" s="165"/>
       <c r="J27" s="34"/>
       <c r="L27" s="97"/>
       <c r="IT27" s="2"/>
     </row>
     <row r="28" spans="1:254" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A28" s="29"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="164"/>
+      <c r="B28" s="163"/>
+      <c r="C28" s="164"/>
+      <c r="D28" s="164"/>
+      <c r="E28" s="164"/>
+      <c r="F28" s="164"/>
+      <c r="G28" s="164"/>
+      <c r="H28" s="164"/>
+      <c r="I28" s="165"/>
       <c r="J28" s="34"/>
       <c r="IT28" s="2"/>
     </row>
     <row r="29" spans="1:254" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A29" s="29"/>
-      <c r="B29" s="162"/>
-      <c r="C29" s="163"/>
-      <c r="D29" s="163"/>
-      <c r="E29" s="163"/>
-      <c r="F29" s="163"/>
-      <c r="G29" s="163"/>
-      <c r="H29" s="163"/>
-      <c r="I29" s="164"/>
+      <c r="B29" s="163"/>
+      <c r="C29" s="164"/>
+      <c r="D29" s="164"/>
+      <c r="E29" s="164"/>
+      <c r="F29" s="164"/>
+      <c r="G29" s="164"/>
+      <c r="H29" s="164"/>
+      <c r="I29" s="165"/>
       <c r="J29" s="34"/>
       <c r="IT29" s="2"/>
     </row>
     <row r="30" spans="1:254" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A30" s="29"/>
-      <c r="B30" s="165"/>
-      <c r="C30" s="166"/>
-      <c r="D30" s="166"/>
-      <c r="E30" s="166"/>
-      <c r="F30" s="166"/>
-      <c r="G30" s="166"/>
-      <c r="H30" s="166"/>
-      <c r="I30" s="167"/>
+      <c r="B30" s="166"/>
+      <c r="C30" s="167"/>
+      <c r="D30" s="167"/>
+      <c r="E30" s="167"/>
+      <c r="F30" s="167"/>
+      <c r="G30" s="167"/>
+      <c r="H30" s="167"/>
+      <c r="I30" s="168"/>
       <c r="J30" s="34"/>
       <c r="IT30" s="2"/>
     </row>

</xml_diff>